<commit_message>
Add a tile and makefile
</commit_message>
<xml_diff>
--- a/ref/TileEditor.xlsx
+++ b/ref/TileEditor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\sokoban\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE400C2-BD2F-4306-B488-007D8825334D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E853350E-878A-4D86-91ED-21BAA63EC0D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F168D399-CC1E-4221-8254-6D6798085CB3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{F168D399-CC1E-4221-8254-6D6798085CB3}"/>
   </bookViews>
   <sheets>
     <sheet name="Visual" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,10 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -64,12 +68,92 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -78,22 +162,39 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -433,58 +534,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E3C335D-9A4B-4AD1-9E0A-380A94C73AA5}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="A1:H8"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="2.33203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>1</v>
-      </c>
-      <c r="E1">
-        <v>1</v>
-      </c>
-      <c r="F1">
-        <v>1</v>
-      </c>
-      <c r="G1">
-        <v>1</v>
-      </c>
-      <c r="H1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>1</v>
-      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
       <c r="B4">
         <v>1</v>
       </c>
@@ -503,15 +594,10 @@
       <c r="G4">
         <v>1</v>
       </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
         <v>1</v>
       </c>
       <c r="C5">
@@ -523,55 +609,51 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B6">
+      <c r="H5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
         <v>1</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="6"/>
+      <c r="B8" s="7">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7">
+        <v>1</v>
+      </c>
+      <c r="H8" s="8">
         <v>1</v>
       </c>
     </row>
@@ -593,20 +675,20 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1">
         <f>Visual!A1</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1">
         <f>Visual!B1</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1">
         <f>Visual!C1</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1">
         <f>Visual!D1</f>
@@ -622,14 +704,14 @@
       </c>
       <c r="G1">
         <f>Visual!G1</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H1">
         <f>Visual!H1</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>Visual!A2</f>
         <v>0</v>
@@ -652,7 +734,7 @@
       </c>
       <c r="F2">
         <f>Visual!F2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <f>Visual!G2</f>
@@ -660,10 +742,10 @@
       </c>
       <c r="H2">
         <f>Visual!H2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>Visual!A3</f>
         <v>0</v>
@@ -682,7 +764,7 @@
       </c>
       <c r="E3">
         <f>Visual!E3</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <f>Visual!F3</f>
@@ -694,13 +776,13 @@
       </c>
       <c r="H3">
         <f>Visual!H3</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>Visual!A4</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4">
         <f>Visual!B4</f>
@@ -728,17 +810,17 @@
       </c>
       <c r="H4">
         <f>Visual!H4</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>Visual!A5</f>
         <v>1</v>
       </c>
       <c r="B5">
         <f>Visual!B5</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <f>Visual!C5</f>
@@ -754,37 +836,37 @@
       </c>
       <c r="F5">
         <f>Visual!F5</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <f>Visual!G5</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <f>Visual!H5</f>
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <f>Visual!A6</f>
         <v>0</v>
       </c>
       <c r="B6">
         <f>Visual!B6</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <f>Visual!C6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <f>Visual!D6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <f>Visual!E6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <f>Visual!F6</f>
@@ -799,7 +881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>Visual!A7</f>
         <v>0</v>
@@ -822,21 +904,21 @@
       </c>
       <c r="F7">
         <f>Visual!F7</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <f>Visual!G7</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <f>Visual!H7</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <f>Visual!A8</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8">
         <f>Visual!B8</f>
@@ -848,15 +930,15 @@
       </c>
       <c r="D8">
         <f>Visual!D8</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <f>Visual!E8</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <f>Visual!F8</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <f>Visual!G8</f>
@@ -882,54 +964,54 @@
       <selection sqref="A1:A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="str">
         <f>_xlfn.CONCAT("DB %",Binary!A1:H1)</f>
-        <v>DB %11111111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+        <v>DB %00011100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>_xlfn.CONCAT("DB %",Binary!A2:H2)</f>
-        <v>DB %00010001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+        <v>DB %00010100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>_xlfn.CONCAT("DB %",Binary!A3:H3)</f>
-        <v>DB %00010001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+        <v>DB %00011000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>_xlfn.CONCAT("DB %",Binary!A4:H4)</f>
-        <v>DB %11111111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+        <v>DB %01111110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f>_xlfn.CONCAT("DB %",Binary!A5:H5)</f>
-        <v>DB %11111111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+        <v>DB %10111001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f>_xlfn.CONCAT("DB %",Binary!A6:H6)</f>
-        <v>DB %01000100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+        <v>DB %00111100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f>_xlfn.CONCAT("DB %",Binary!A7:H7)</f>
-        <v>DB %01000100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+        <v>DB %01000010</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f>_xlfn.CONCAT("DB %",Binary!A8:H8)</f>
-        <v>DB %11111111</v>
+        <v>DB %01100011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Makefile and level2asm.py for improved build process and output clarity; modify tile data in data.nolevels.asm
</commit_message>
<xml_diff>
--- a/ref/TileEditor.xlsx
+++ b/ref/TileEditor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\sokoban\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E853350E-878A-4D86-91ED-21BAA63EC0D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DB19C2-412E-4E34-BD74-84D66BAB4C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{F168D399-CC1E-4221-8254-6D6798085CB3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F168D399-CC1E-4221-8254-6D6798085CB3}"/>
   </bookViews>
   <sheets>
     <sheet name="Visual" sheetId="1" r:id="rId1"/>
@@ -35,10 +35,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -534,14 +530,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E3C335D-9A4B-4AD1-9E0A-380A94C73AA5}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.33203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="2.375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
+        <v>1</v>
+      </c>
       <c r="D1" s="2">
         <v>1</v>
       </c>
@@ -551,71 +555,59 @@
       <c r="F1" s="2">
         <v>1</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G1" s="2">
+        <v>1</v>
+      </c>
+      <c r="H1" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>1</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
+      <c r="F5">
         <v>1</v>
       </c>
       <c r="H5" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="C6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
         <v>1</v>
       </c>
       <c r="D6">
@@ -624,32 +616,37 @@
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
+      <c r="H6" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>1</v>
+      </c>
+      <c r="H7" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <v>1</v>
+      </c>
       <c r="B8" s="7">
         <v>1</v>
       </c>
       <c r="C8" s="7">
         <v>1</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7">
+        <v>1</v>
+      </c>
       <c r="G8" s="7">
         <v>1</v>
       </c>
@@ -675,20 +672,20 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1">
         <f>Visual!A1</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1">
         <f>Visual!B1</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1">
         <f>Visual!C1</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1">
         <f>Visual!D1</f>
@@ -704,17 +701,17 @@
       </c>
       <c r="G1">
         <f>Visual!G1</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1">
         <f>Visual!H1</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>Visual!A2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <f>Visual!B2</f>
@@ -726,7 +723,7 @@
       </c>
       <c r="D2">
         <f>Visual!D2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <f>Visual!E2</f>
@@ -734,7 +731,7 @@
       </c>
       <c r="F2">
         <f>Visual!F2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <f>Visual!G2</f>
@@ -742,13 +739,13 @@
       </c>
       <c r="H2">
         <f>Visual!H2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>Visual!A3</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <f>Visual!B3</f>
@@ -756,19 +753,19 @@
       </c>
       <c r="C3">
         <f>Visual!C3</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <f>Visual!D3</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <f>Visual!E3</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <f>Visual!F3</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <f>Visual!G3</f>
@@ -776,44 +773,44 @@
       </c>
       <c r="H3">
         <f>Visual!H3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <f>Visual!A4</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <f>Visual!B4</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <f>Visual!C4</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <f>Visual!D4</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <f>Visual!E4</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <f>Visual!F4</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <f>Visual!G4</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <f>Visual!H4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <f>Visual!A5</f>
         <v>1</v>
@@ -828,15 +825,15 @@
       </c>
       <c r="D5">
         <f>Visual!D5</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <f>Visual!E5</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <f>Visual!F5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <f>Visual!G5</f>
@@ -847,10 +844,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <f>Visual!A6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6">
         <f>Visual!B6</f>
@@ -858,7 +855,7 @@
       </c>
       <c r="C6">
         <f>Visual!C6</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <f>Visual!D6</f>
@@ -870,7 +867,7 @@
       </c>
       <c r="F6">
         <f>Visual!F6</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <f>Visual!G6</f>
@@ -878,17 +875,17 @@
       </c>
       <c r="H6">
         <f>Visual!H6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <f>Visual!A7</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7">
         <f>Visual!B7</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <f>Visual!C7</f>
@@ -908,17 +905,17 @@
       </c>
       <c r="G7">
         <f>Visual!G7</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7">
         <f>Visual!H7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <f>Visual!A8</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B8">
         <f>Visual!B8</f>
@@ -930,15 +927,15 @@
       </c>
       <c r="D8">
         <f>Visual!D8</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <f>Visual!E8</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <f>Visual!F8</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <f>Visual!G8</f>
@@ -964,58 +961,59 @@
       <selection sqref="A1:A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
         <f>_xlfn.CONCAT("DB %",Binary!A1:H1)</f>
-        <v>DB %00011100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+        <v>DB %11111111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>_xlfn.CONCAT("DB %",Binary!A2:H2)</f>
-        <v>DB %00010100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+        <v>DB %10000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>_xlfn.CONCAT("DB %",Binary!A3:H3)</f>
-        <v>DB %00011000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+        <v>DB %10100101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f>_xlfn.CONCAT("DB %",Binary!A4:H4)</f>
-        <v>DB %01111110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+        <v>DB %10000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f>_xlfn.CONCAT("DB %",Binary!A5:H5)</f>
-        <v>DB %10111001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+        <v>DB %10100101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f>_xlfn.CONCAT("DB %",Binary!A6:H6)</f>
-        <v>DB %00111100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+        <v>DB %10011001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f>_xlfn.CONCAT("DB %",Binary!A7:H7)</f>
-        <v>DB %01000010</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+        <v>DB %10000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f>_xlfn.CONCAT("DB %",Binary!A8:H8)</f>
-        <v>DB %01100011</v>
+        <v>DB %11111111</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>